<commit_message>
update mau setor 10 juni 2021
</commit_message>
<xml_diff>
--- a/4. PDH DP 3N30 (MERAH) 3T25(COKLAT MUDA) 4N31(PUTIH) 5N38(HIJAU TUA) 5T38(PINKMUDA)/DP5NT38.xlsx
+++ b/4. PDH DP 3N30 (MERAH) 3T25(COKLAT MUDA) 4N31(PUTIH) 5N38(HIJAU TUA) 5T38(PINKMUDA)/DP5NT38.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\4. PDH DP 3N30 (MERAH) 3T25(COKLAT MUDA) 4N31(PUTIH) 5N38(HIJAU TUA) 5T38(PINKMUDA)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664D77D5-E509-4AAE-A7C5-66C30390369E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF44473-60DC-495A-8DE9-13323480E5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{648D9222-A383-4770-A314-359676E95833}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="7965" xr2:uid="{648D9222-A383-4770-A314-359676E95833}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="142">
   <si>
     <t>KELAS</t>
   </si>
@@ -436,6 +436,21 @@
   </si>
   <si>
     <t>TOPI</t>
+  </si>
+  <si>
+    <t>wanita</t>
+  </si>
+  <si>
+    <t>dp5nt38</t>
+  </si>
+  <si>
+    <t>dp3t24</t>
+  </si>
+  <si>
+    <t>dp3t26</t>
+  </si>
+  <si>
+    <t>jml</t>
   </si>
 </sst>
 </file>
@@ -501,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -520,6 +535,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -835,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E239AF7-B0E1-41C1-A6A5-DDF7A97D9254}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -851,7 +869,7 @@
     <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>133</v>
       </c>
@@ -867,8 +885,20 @@
       <c r="E1" s="4" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
@@ -884,8 +914,18 @@
       <c r="E2" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="3">
+        <v>38</v>
+      </c>
+      <c r="K2" s="3">
+        <v>2</v>
+      </c>
+      <c r="L2" s="3">
+        <f>SUM(J2:K2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -901,8 +941,25 @@
       <c r="E3" s="5">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="5">
+        <v>39</v>
+      </c>
+      <c r="J3" s="3">
+        <f>COUNTIF(D2:$D$66,I3)</f>
+        <v>5</v>
+      </c>
+      <c r="K3" s="3">
+        <v>2</v>
+      </c>
+      <c r="L3" s="3">
+        <f t="shared" ref="L3:L10" si="0">SUM(J3:K3)</f>
+        <v>7</v>
+      </c>
+      <c r="P3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -918,8 +975,25 @@
       <c r="E4" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="5">
+        <v>40</v>
+      </c>
+      <c r="J4" s="3">
+        <f>COUNTIF(D3:$D$66,I4)</f>
+        <v>8</v>
+      </c>
+      <c r="K4" s="3">
+        <v>6</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="P4" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -935,8 +1009,25 @@
       <c r="E5" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="5">
+        <v>41</v>
+      </c>
+      <c r="J5" s="3">
+        <f>COUNTIF(D4:$D$66,I5)</f>
+        <v>14</v>
+      </c>
+      <c r="K5" s="3">
+        <v>9</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="P5" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
@@ -952,8 +1043,25 @@
       <c r="E6" s="5">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="5">
+        <v>42</v>
+      </c>
+      <c r="J6" s="3">
+        <f>COUNTIF(D5:$D$66,I6)</f>
+        <v>24</v>
+      </c>
+      <c r="K6" s="3">
+        <v>12</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="P6" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -969,8 +1077,25 @@
       <c r="E7" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="5">
+        <v>43</v>
+      </c>
+      <c r="J7" s="3">
+        <f>COUNTIF(D6:$D$66,I7)</f>
+        <v>8</v>
+      </c>
+      <c r="K7" s="3">
+        <v>10</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="P7" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -986,8 +1111,25 @@
       <c r="E8" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="5">
+        <v>44</v>
+      </c>
+      <c r="J8" s="3">
+        <f>COUNTIF(D7:$D$66,I8)</f>
+        <v>1</v>
+      </c>
+      <c r="K8" s="3">
+        <v>2</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="P8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -1003,8 +1145,22 @@
       <c r="E9" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="5">
+        <v>45</v>
+      </c>
+      <c r="J9" s="3">
+        <f>COUNTIF(D8:$D$66,I9)</f>
+        <v>1</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
@@ -1020,8 +1176,25 @@
       <c r="E10" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10"/>
+      <c r="J10" s="3">
+        <f>SUM(J3:J9)</f>
+        <v>61</v>
+      </c>
+      <c r="K10" s="3">
+        <f>SUM(K2:K9)</f>
+        <v>43</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+      <c r="P10" s="3">
+        <f>SUM(P3:P9)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
@@ -1037,8 +1210,11 @@
       <c r="E11" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
@@ -1054,8 +1230,14 @@
       <c r="E12" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="7">
+        <v>38</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
@@ -1071,8 +1253,14 @@
       <c r="E13" s="5">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="7">
+        <v>44</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
@@ -1088,8 +1276,9 @@
       <c r="E14" s="5">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I14"/>
+    </row>
+    <row r="15" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
@@ -1105,8 +1294,9 @@
       <c r="E15" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I15"/>
+    </row>
+    <row r="16" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>29</v>
       </c>
@@ -1122,8 +1312,9 @@
       <c r="E16" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16"/>
+    </row>
+    <row r="17" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>30</v>
       </c>
@@ -1139,8 +1330,9 @@
       <c r="E17" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17"/>
+    </row>
+    <row r="18" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>31</v>
       </c>
@@ -1156,8 +1348,9 @@
       <c r="E18" s="5">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18"/>
+    </row>
+    <row r="19" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
@@ -1173,8 +1366,9 @@
       <c r="E19" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I19"/>
+    </row>
+    <row r="20" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>33</v>
       </c>
@@ -1190,8 +1384,9 @@
       <c r="E20" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20"/>
+    </row>
+    <row r="21" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>34</v>
       </c>
@@ -1207,8 +1402,9 @@
       <c r="E21" s="5">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21"/>
+    </row>
+    <row r="22" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>35</v>
       </c>
@@ -1224,8 +1420,9 @@
       <c r="E22" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I22"/>
+    </row>
+    <row r="23" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>36</v>
       </c>
@@ -1241,8 +1438,9 @@
       <c r="E23" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23"/>
+    </row>
+    <row r="24" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>37</v>
       </c>
@@ -1258,8 +1456,9 @@
       <c r="E24" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24"/>
+    </row>
+    <row r="25" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
@@ -1275,8 +1474,9 @@
       <c r="E25" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I25"/>
+    </row>
+    <row r="26" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>39</v>
       </c>
@@ -1292,8 +1492,9 @@
       <c r="E26" s="5">
         <v>54</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I26"/>
+    </row>
+    <row r="27" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>40</v>
       </c>
@@ -1309,8 +1510,9 @@
       <c r="E27" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I27"/>
+    </row>
+    <row r="28" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>41</v>
       </c>
@@ -1326,8 +1528,9 @@
       <c r="E28" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I28"/>
+    </row>
+    <row r="29" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>42</v>
       </c>
@@ -1343,8 +1546,9 @@
       <c r="E29" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I29"/>
+    </row>
+    <row r="30" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>43</v>
       </c>
@@ -1360,8 +1564,9 @@
       <c r="E30" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I30"/>
+    </row>
+    <row r="31" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>44</v>
       </c>
@@ -1377,8 +1582,9 @@
       <c r="E31" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I31"/>
+    </row>
+    <row r="32" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>45</v>
       </c>
@@ -1394,8 +1600,9 @@
       <c r="E32" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I32"/>
+    </row>
+    <row r="33" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>46</v>
       </c>
@@ -1411,8 +1618,9 @@
       <c r="E33" s="5">
         <v>58</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I33"/>
+    </row>
+    <row r="34" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>47</v>
       </c>
@@ -1428,8 +1636,9 @@
       <c r="E34" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I34"/>
+    </row>
+    <row r="35" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>48</v>
       </c>
@@ -1445,8 +1654,9 @@
       <c r="E35" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I35"/>
+    </row>
+    <row r="36" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>49</v>
       </c>
@@ -1462,8 +1672,9 @@
       <c r="E36" s="5">
         <v>53</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I36"/>
+    </row>
+    <row r="37" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>72</v>
       </c>
@@ -1479,8 +1690,9 @@
       <c r="E37" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I37"/>
+    </row>
+    <row r="38" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>73</v>
       </c>
@@ -1496,8 +1708,9 @@
       <c r="E38" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I38"/>
+    </row>
+    <row r="39" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>74</v>
       </c>
@@ -1513,8 +1726,9 @@
       <c r="E39" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I39"/>
+    </row>
+    <row r="40" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>75</v>
       </c>
@@ -1530,8 +1744,9 @@
       <c r="E40" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I40"/>
+    </row>
+    <row r="41" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>76</v>
       </c>
@@ -1547,8 +1762,9 @@
       <c r="E41" s="5">
         <v>54</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I41"/>
+    </row>
+    <row r="42" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>77</v>
       </c>
@@ -1564,8 +1780,9 @@
       <c r="E42" s="5">
         <v>54</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I42"/>
+    </row>
+    <row r="43" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>78</v>
       </c>
@@ -1581,8 +1798,9 @@
       <c r="E43" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I43"/>
+    </row>
+    <row r="44" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>79</v>
       </c>
@@ -1598,8 +1816,9 @@
       <c r="E44" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I44"/>
+    </row>
+    <row r="45" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>80</v>
       </c>
@@ -1615,8 +1834,9 @@
       <c r="E45" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I45"/>
+    </row>
+    <row r="46" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>81</v>
       </c>
@@ -1632,8 +1852,9 @@
       <c r="E46" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I46"/>
+    </row>
+    <row r="47" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>82</v>
       </c>
@@ -1649,8 +1870,9 @@
       <c r="E47" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I47"/>
+    </row>
+    <row r="48" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>83</v>
       </c>
@@ -1666,8 +1888,9 @@
       <c r="E48" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I48"/>
+    </row>
+    <row r="49" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>84</v>
       </c>
@@ -1683,8 +1906,9 @@
       <c r="E49" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I49"/>
+    </row>
+    <row r="50" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>85</v>
       </c>
@@ -1700,8 +1924,9 @@
       <c r="E50" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I50"/>
+    </row>
+    <row r="51" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>86</v>
       </c>
@@ -1717,8 +1942,9 @@
       <c r="E51" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I51"/>
+    </row>
+    <row r="52" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>87</v>
       </c>
@@ -1734,8 +1960,9 @@
       <c r="E52" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I52"/>
+    </row>
+    <row r="53" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>88</v>
       </c>
@@ -1751,8 +1978,9 @@
       <c r="E53" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I53"/>
+    </row>
+    <row r="54" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>89</v>
       </c>
@@ -1768,8 +1996,9 @@
       <c r="E54" s="5">
         <v>59</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I54"/>
+    </row>
+    <row r="55" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>90</v>
       </c>
@@ -1785,8 +2014,9 @@
       <c r="E55" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I55"/>
+    </row>
+    <row r="56" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>91</v>
       </c>
@@ -1802,8 +2032,9 @@
       <c r="E56" s="5">
         <v>58</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I56"/>
+    </row>
+    <row r="57" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>92</v>
       </c>
@@ -1819,8 +2050,9 @@
       <c r="E57" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I57"/>
+    </row>
+    <row r="58" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>93</v>
       </c>
@@ -1836,8 +2068,9 @@
       <c r="E58" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I58"/>
+    </row>
+    <row r="59" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>94</v>
       </c>
@@ -1853,8 +2086,9 @@
       <c r="E59" s="5">
         <v>54</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I59"/>
+    </row>
+    <row r="60" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>95</v>
       </c>
@@ -1870,8 +2104,9 @@
       <c r="E60" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I60"/>
+    </row>
+    <row r="61" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>96</v>
       </c>
@@ -1887,8 +2122,9 @@
       <c r="E61" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I61"/>
+    </row>
+    <row r="62" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>97</v>
       </c>
@@ -1904,8 +2140,9 @@
       <c r="E62" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I62"/>
+    </row>
+    <row r="63" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>98</v>
       </c>
@@ -1921,8 +2158,9 @@
       <c r="E63" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I63"/>
+    </row>
+    <row r="64" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>99</v>
       </c>
@@ -1938,8 +2176,9 @@
       <c r="E64" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I64"/>
+    </row>
+    <row r="65" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>100</v>
       </c>
@@ -1955,8 +2194,9 @@
       <c r="E65" s="5">
         <v>58</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I65"/>
+    </row>
+    <row r="66" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>101</v>
       </c>
@@ -1972,8 +2212,12 @@
       <c r="E66" s="5">
         <v>58</v>
       </c>
+      <c r="I66"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I2:I66">
+    <sortCondition ref="I2:I66"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.57999999999999996" bottom="0.15" header="0.3" footer="0.12"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>